<commit_message>
Atualização de bases das ligas, do dia: 28-05-2024 às 20:56
</commit_message>
<xml_diff>
--- a/Austria 2 Liga/Austria 2 Liga.xlsx
+++ b/Austria 2 Liga/Austria 2 Liga.xlsx
@@ -2750,7 +2750,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6832846</v>
+        <v>6832850</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -2759,55 +2759,55 @@
         <v>45149.54861111111</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L25">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="M25">
         <v>3.6</v>
       </c>
       <c r="N25">
-        <v>3.8</v>
+        <v>1.85</v>
       </c>
       <c r="O25">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="P25">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="Q25">
-        <v>6</v>
+        <v>2.05</v>
       </c>
       <c r="R25">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="S25">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T25">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U25">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="V25">
         <v>1.825</v>
@@ -2816,19 +2816,19 @@
         <v>1.975</v>
       </c>
       <c r="X25">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Y25">
         <v>-1</v>
       </c>
       <c r="Z25">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AA25">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AB25">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC25">
         <v>-1</v>
@@ -2842,7 +2842,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6832849</v>
+        <v>6832846</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
@@ -2851,82 +2851,82 @@
         <v>45149.54861111111</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L26">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="M26">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="N26">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="O26">
-        <v>1.909</v>
+        <v>1.5</v>
       </c>
       <c r="P26">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="Q26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R26">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="S26">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="T26">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="U26">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="V26">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W26">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="X26">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="Y26">
         <v>-1</v>
       </c>
       <c r="Z26">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AA26">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB26">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC26">
         <v>-1</v>
       </c>
       <c r="AD26">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:30">
@@ -2934,7 +2934,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6832850</v>
+        <v>6832849</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
@@ -2943,10 +2943,10 @@
         <v>45149.54861111111</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2964,43 +2964,43 @@
         <v>50</v>
       </c>
       <c r="L27">
-        <v>3.6</v>
+        <v>2.05</v>
       </c>
       <c r="M27">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="N27">
-        <v>1.85</v>
+        <v>3.2</v>
       </c>
       <c r="O27">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="P27">
         <v>3.6</v>
       </c>
       <c r="Q27">
-        <v>2.05</v>
+        <v>4</v>
       </c>
       <c r="R27">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="S27">
-        <v>1.75</v>
+        <v>1.875</v>
       </c>
       <c r="T27">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U27">
         <v>2.75</v>
       </c>
       <c r="V27">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W27">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="X27">
-        <v>2.3</v>
+        <v>0.909</v>
       </c>
       <c r="Y27">
         <v>-1</v>
@@ -3009,7 +3009,7 @@
         <v>-1</v>
       </c>
       <c r="AA27">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="AB27">
         <v>-1</v>
@@ -3018,7 +3018,7 @@
         <v>-1</v>
       </c>
       <c r="AD27">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -11030,7 +11030,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>6832905</v>
+        <v>6832904</v>
       </c>
       <c r="C115" t="s">
         <v>29</v>
@@ -11039,10 +11039,10 @@
         <v>45240.59027777778</v>
       </c>
       <c r="E115" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F115" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G115">
         <v>2</v>
@@ -11051,7 +11051,7 @@
         <v>1</v>
       </c>
       <c r="I115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J115">
         <v>1</v>
@@ -11060,43 +11060,43 @@
         <v>50</v>
       </c>
       <c r="L115">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="M115">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="N115">
-        <v>4.2</v>
+        <v>2.5</v>
       </c>
       <c r="O115">
-        <v>1.4</v>
+        <v>2.55</v>
       </c>
       <c r="P115">
-        <v>5.25</v>
+        <v>3.25</v>
       </c>
       <c r="Q115">
-        <v>7</v>
+        <v>2.875</v>
       </c>
       <c r="R115">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="S115">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T115">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="U115">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="V115">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="W115">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="X115">
-        <v>0.3999999999999999</v>
+        <v>1.55</v>
       </c>
       <c r="Y115">
         <v>-1</v>
@@ -11105,16 +11105,16 @@
         <v>-1</v>
       </c>
       <c r="AA115">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB115">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC115">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD115">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="116" spans="1:30">
@@ -11122,7 +11122,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>6832904</v>
+        <v>6832905</v>
       </c>
       <c r="C116" t="s">
         <v>29</v>
@@ -11131,10 +11131,10 @@
         <v>45240.59027777778</v>
       </c>
       <c r="E116" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F116" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G116">
         <v>2</v>
@@ -11143,7 +11143,7 @@
         <v>1</v>
       </c>
       <c r="I116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J116">
         <v>1</v>
@@ -11152,43 +11152,43 @@
         <v>50</v>
       </c>
       <c r="L116">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="M116">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="N116">
-        <v>2.5</v>
+        <v>4.2</v>
       </c>
       <c r="O116">
-        <v>2.55</v>
+        <v>1.4</v>
       </c>
       <c r="P116">
-        <v>3.25</v>
+        <v>5.25</v>
       </c>
       <c r="Q116">
-        <v>2.875</v>
+        <v>7</v>
       </c>
       <c r="R116">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="S116">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="T116">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="U116">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="V116">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W116">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="X116">
-        <v>1.55</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Y116">
         <v>-1</v>
@@ -11197,16 +11197,16 @@
         <v>-1</v>
       </c>
       <c r="AA116">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB116">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC116">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD116">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="117" spans="1:30">
@@ -11858,7 +11858,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>6832908</v>
+        <v>6832911</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11867,61 +11867,61 @@
         <v>45255.4375</v>
       </c>
       <c r="E124" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F124" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K124" t="s">
         <v>52</v>
       </c>
       <c r="L124">
-        <v>2.2</v>
+        <v>5.75</v>
       </c>
       <c r="M124">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="N124">
-        <v>2.75</v>
+        <v>1.444</v>
       </c>
       <c r="O124">
-        <v>2.375</v>
+        <v>7.5</v>
       </c>
       <c r="P124">
-        <v>3.75</v>
+        <v>5.25</v>
       </c>
       <c r="Q124">
-        <v>2.7</v>
+        <v>1.363</v>
       </c>
       <c r="R124">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="S124">
-        <v>1.775</v>
+        <v>1.85</v>
       </c>
       <c r="T124">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="U124">
         <v>3</v>
       </c>
       <c r="V124">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W124">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="X124">
         <v>-1</v>
@@ -11930,19 +11930,19 @@
         <v>-1</v>
       </c>
       <c r="Z124">
-        <v>1.7</v>
+        <v>0.363</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>1.025</v>
+        <v>0.95</v>
       </c>
       <c r="AC124">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD124">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11950,7 +11950,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>6832911</v>
+        <v>6832092</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11959,19 +11959,19 @@
         <v>45255.4375</v>
       </c>
       <c r="E125" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F125" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J125">
         <v>1</v>
@@ -11980,40 +11980,40 @@
         <v>52</v>
       </c>
       <c r="L125">
-        <v>5.75</v>
+        <v>1.909</v>
       </c>
       <c r="M125">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="N125">
-        <v>1.444</v>
+        <v>3.6</v>
       </c>
       <c r="O125">
-        <v>7.5</v>
+        <v>2.15</v>
       </c>
       <c r="P125">
-        <v>5.25</v>
+        <v>3.25</v>
       </c>
       <c r="Q125">
-        <v>1.363</v>
+        <v>3.4</v>
       </c>
       <c r="R125">
-        <v>1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S125">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T125">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="U125">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="V125">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="W125">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="X125">
         <v>-1</v>
@@ -12022,19 +12022,19 @@
         <v>-1</v>
       </c>
       <c r="Z125">
-        <v>0.363</v>
+        <v>2.4</v>
       </c>
       <c r="AA125">
         <v>-1</v>
       </c>
       <c r="AB125">
-        <v>0.95</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC125">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AD125">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="126" spans="1:30">
@@ -12042,7 +12042,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>6832092</v>
+        <v>6832908</v>
       </c>
       <c r="C126" t="s">
         <v>29</v>
@@ -12051,61 +12051,61 @@
         <v>45255.4375</v>
       </c>
       <c r="E126" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F126" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G126">
         <v>1</v>
       </c>
       <c r="H126">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J126">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K126" t="s">
         <v>52</v>
       </c>
       <c r="L126">
-        <v>1.909</v>
+        <v>2.2</v>
       </c>
       <c r="M126">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="N126">
-        <v>3.6</v>
+        <v>2.75</v>
       </c>
       <c r="O126">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="P126">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q126">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="R126">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="S126">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="T126">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="U126">
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="V126">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W126">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="X126">
         <v>-1</v>
@@ -12114,16 +12114,16 @@
         <v>-1</v>
       </c>
       <c r="Z126">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="AA126">
         <v>-1</v>
       </c>
       <c r="AB126">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AC126">
-        <v>0.875</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD126">
         <v>-1</v>
@@ -13882,7 +13882,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>6832097</v>
+        <v>6832929</v>
       </c>
       <c r="C146" t="s">
         <v>29</v>
@@ -13891,16 +13891,16 @@
         <v>45352.59027777778</v>
       </c>
       <c r="E146" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F146" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I146">
         <v>0</v>
@@ -13909,64 +13909,64 @@
         <v>0</v>
       </c>
       <c r="K146" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L146">
-        <v>3.6</v>
+        <v>1.3</v>
       </c>
       <c r="M146">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="N146">
-        <v>1.833</v>
+        <v>7.5</v>
       </c>
       <c r="O146">
-        <v>4</v>
+        <v>1.363</v>
       </c>
       <c r="P146">
-        <v>4</v>
+        <v>5.25</v>
       </c>
       <c r="Q146">
-        <v>1.8</v>
+        <v>7</v>
       </c>
       <c r="R146">
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="S146">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="T146">
-        <v>1.775</v>
+        <v>1.825</v>
       </c>
       <c r="U146">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V146">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W146">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="X146">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="Y146">
         <v>-1</v>
       </c>
       <c r="Z146">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA146">
         <v>-1</v>
       </c>
       <c r="AB146">
-        <v>0.7749999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AC146">
         <v>-1</v>
       </c>
       <c r="AD146">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="147" spans="1:30">
@@ -13974,7 +13974,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>6832926</v>
+        <v>6832097</v>
       </c>
       <c r="C147" t="s">
         <v>29</v>
@@ -13983,82 +13983,82 @@
         <v>45352.59027777778</v>
       </c>
       <c r="E147" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F147" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G147">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J147">
         <v>0</v>
       </c>
       <c r="K147" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L147">
-        <v>1.5</v>
+        <v>3.6</v>
       </c>
       <c r="M147">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="N147">
-        <v>5</v>
+        <v>1.833</v>
       </c>
       <c r="O147">
-        <v>1.363</v>
+        <v>4</v>
       </c>
       <c r="P147">
-        <v>5.25</v>
+        <v>4</v>
       </c>
       <c r="Q147">
-        <v>7</v>
+        <v>1.8</v>
       </c>
       <c r="R147">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="S147">
+        <v>2.025</v>
+      </c>
+      <c r="T147">
+        <v>1.775</v>
+      </c>
+      <c r="U147">
+        <v>2.5</v>
+      </c>
+      <c r="V147">
         <v>1.8</v>
       </c>
-      <c r="T147">
-        <v>2</v>
-      </c>
-      <c r="U147">
-        <v>3</v>
-      </c>
-      <c r="V147">
-        <v>1.95</v>
-      </c>
       <c r="W147">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="X147">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="Y147">
         <v>-1</v>
       </c>
       <c r="Z147">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA147">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB147">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AC147">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD147">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:30">
@@ -14066,7 +14066,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>6832929</v>
+        <v>6832926</v>
       </c>
       <c r="C148" t="s">
         <v>29</v>
@@ -14075,19 +14075,19 @@
         <v>45352.59027777778</v>
       </c>
       <c r="E148" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F148" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G148">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H148">
         <v>0</v>
       </c>
       <c r="I148">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J148">
         <v>0</v>
@@ -14096,13 +14096,13 @@
         <v>50</v>
       </c>
       <c r="L148">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="M148">
+        <v>4.2</v>
+      </c>
+      <c r="N148">
         <v>5</v>
-      </c>
-      <c r="N148">
-        <v>7.5</v>
       </c>
       <c r="O148">
         <v>1.363</v>
@@ -14114,22 +14114,22 @@
         <v>7</v>
       </c>
       <c r="R148">
-        <v>-1.5</v>
+        <v>-1.25</v>
       </c>
       <c r="S148">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="T148">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="U148">
         <v>3</v>
       </c>
       <c r="V148">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W148">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="X148">
         <v>0.363</v>
@@ -14141,16 +14141,16 @@
         <v>-1</v>
       </c>
       <c r="AA148">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB148">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC148">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AD148">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="149" spans="1:30">
@@ -15354,7 +15354,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>6832100</v>
+        <v>6832935</v>
       </c>
       <c r="C162" t="s">
         <v>29</v>
@@ -15363,82 +15363,82 @@
         <v>45366.59027777778</v>
       </c>
       <c r="E162" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F162" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G162">
         <v>1</v>
       </c>
       <c r="H162">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K162" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L162">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
       <c r="M162">
+        <v>3.5</v>
+      </c>
+      <c r="N162">
+        <v>2</v>
+      </c>
+      <c r="O162">
+        <v>3.2</v>
+      </c>
+      <c r="P162">
         <v>3.3</v>
       </c>
-      <c r="N162">
-        <v>2.4</v>
-      </c>
-      <c r="O162">
-        <v>3.75</v>
-      </c>
-      <c r="P162">
-        <v>3.25</v>
-      </c>
       <c r="Q162">
-        <v>2.1</v>
+        <v>2.25</v>
       </c>
       <c r="R162">
         <v>0.25</v>
       </c>
       <c r="S162">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="T162">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U162">
         <v>2.25</v>
       </c>
       <c r="V162">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="W162">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="X162">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y162">
         <v>-1</v>
       </c>
       <c r="Z162">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="AA162">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB162">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC162">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD162">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="163" spans="1:30">
@@ -15446,7 +15446,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>6832936</v>
+        <v>6832939</v>
       </c>
       <c r="C163" t="s">
         <v>29</v>
@@ -15455,64 +15455,64 @@
         <v>45366.59027777778</v>
       </c>
       <c r="E163" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F163" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K163" t="s">
         <v>50</v>
       </c>
       <c r="L163">
-        <v>1.615</v>
+        <v>2.05</v>
       </c>
       <c r="M163">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="N163">
-        <v>4.75</v>
+        <v>3.1</v>
       </c>
       <c r="O163">
-        <v>1.909</v>
+        <v>2.05</v>
       </c>
       <c r="P163">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="Q163">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="R163">
         <v>-0.5</v>
       </c>
       <c r="S163">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T163">
-        <v>1.925</v>
+        <v>1.75</v>
       </c>
       <c r="U163">
         <v>2.75</v>
       </c>
       <c r="V163">
+        <v>1.925</v>
+      </c>
+      <c r="W163">
         <v>1.875</v>
       </c>
-      <c r="W163">
-        <v>1.925</v>
-      </c>
       <c r="X163">
-        <v>0.909</v>
+        <v>1.05</v>
       </c>
       <c r="Y163">
         <v>-1</v>
@@ -15521,16 +15521,16 @@
         <v>-1</v>
       </c>
       <c r="AA163">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AB163">
         <v>-1</v>
       </c>
       <c r="AC163">
-        <v>0.875</v>
+        <v>0.4625</v>
       </c>
       <c r="AD163">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="164" spans="1:30">
@@ -15538,7 +15538,7 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>6832938</v>
+        <v>6832100</v>
       </c>
       <c r="C164" t="s">
         <v>29</v>
@@ -15547,16 +15547,16 @@
         <v>45366.59027777778</v>
       </c>
       <c r="E164" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F164" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G164">
         <v>1</v>
       </c>
       <c r="H164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I164">
         <v>0</v>
@@ -15565,64 +15565,64 @@
         <v>0</v>
       </c>
       <c r="K164" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L164">
-        <v>1.444</v>
+        <v>2.8</v>
       </c>
       <c r="M164">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="N164">
-        <v>6</v>
+        <v>2.4</v>
       </c>
       <c r="O164">
-        <v>1.4</v>
+        <v>3.75</v>
       </c>
       <c r="P164">
-        <v>4.75</v>
+        <v>3.25</v>
       </c>
       <c r="Q164">
-        <v>7</v>
+        <v>2.1</v>
       </c>
       <c r="R164">
-        <v>-1.25</v>
+        <v>0.25</v>
       </c>
       <c r="S164">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T164">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U164">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="V164">
+        <v>1.85</v>
+      </c>
+      <c r="W164">
         <v>1.95</v>
       </c>
-      <c r="W164">
-        <v>1.85</v>
-      </c>
       <c r="X164">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y164">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Z164">
         <v>-1</v>
       </c>
       <c r="AA164">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB164">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC164">
         <v>-1</v>
       </c>
       <c r="AD164">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="165" spans="1:30">
@@ -15630,7 +15630,7 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>6832939</v>
+        <v>6832936</v>
       </c>
       <c r="C165" t="s">
         <v>29</v>
@@ -15639,64 +15639,64 @@
         <v>45366.59027777778</v>
       </c>
       <c r="E165" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F165" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G165">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K165" t="s">
         <v>50</v>
       </c>
       <c r="L165">
-        <v>2.05</v>
+        <v>1.615</v>
       </c>
       <c r="M165">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="N165">
-        <v>3.1</v>
+        <v>4.75</v>
       </c>
       <c r="O165">
-        <v>2.05</v>
+        <v>1.909</v>
       </c>
       <c r="P165">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="Q165">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="R165">
         <v>-0.5</v>
       </c>
       <c r="S165">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T165">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="U165">
         <v>2.75</v>
       </c>
       <c r="V165">
+        <v>1.875</v>
+      </c>
+      <c r="W165">
         <v>1.925</v>
       </c>
-      <c r="W165">
-        <v>1.875</v>
-      </c>
       <c r="X165">
-        <v>1.05</v>
+        <v>0.909</v>
       </c>
       <c r="Y165">
         <v>-1</v>
@@ -15705,16 +15705,16 @@
         <v>-1</v>
       </c>
       <c r="AA165">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AB165">
         <v>-1</v>
       </c>
       <c r="AC165">
-        <v>0.4625</v>
+        <v>0.875</v>
       </c>
       <c r="AD165">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="166" spans="1:30">
@@ -15722,7 +15722,7 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>6832935</v>
+        <v>6832938</v>
       </c>
       <c r="C166" t="s">
         <v>29</v>
@@ -15731,82 +15731,82 @@
         <v>45366.59027777778</v>
       </c>
       <c r="E166" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F166" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G166">
         <v>1</v>
       </c>
       <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+      <c r="K166" t="s">
+        <v>51</v>
+      </c>
+      <c r="L166">
+        <v>1.444</v>
+      </c>
+      <c r="M166">
+        <v>4.5</v>
+      </c>
+      <c r="N166">
+        <v>6</v>
+      </c>
+      <c r="O166">
+        <v>1.4</v>
+      </c>
+      <c r="P166">
+        <v>4.75</v>
+      </c>
+      <c r="Q166">
+        <v>7</v>
+      </c>
+      <c r="R166">
+        <v>-1.25</v>
+      </c>
+      <c r="S166">
+        <v>1.9</v>
+      </c>
+      <c r="T166">
+        <v>1.9</v>
+      </c>
+      <c r="U166">
         <v>3</v>
       </c>
-      <c r="I166">
-        <v>1</v>
-      </c>
-      <c r="J166">
-        <v>1</v>
-      </c>
-      <c r="K166" t="s">
-        <v>52</v>
-      </c>
-      <c r="L166">
-        <v>3.3</v>
-      </c>
-      <c r="M166">
-        <v>3.5</v>
-      </c>
-      <c r="N166">
-        <v>2</v>
-      </c>
-      <c r="O166">
-        <v>3.2</v>
-      </c>
-      <c r="P166">
-        <v>3.3</v>
-      </c>
-      <c r="Q166">
-        <v>2.25</v>
-      </c>
-      <c r="R166">
-        <v>0.25</v>
-      </c>
-      <c r="S166">
+      <c r="V166">
+        <v>1.95</v>
+      </c>
+      <c r="W166">
         <v>1.85</v>
       </c>
-      <c r="T166">
-        <v>1.95</v>
-      </c>
-      <c r="U166">
-        <v>2.25</v>
-      </c>
-      <c r="V166">
-        <v>1.9</v>
-      </c>
-      <c r="W166">
-        <v>1.9</v>
-      </c>
       <c r="X166">
         <v>-1</v>
       </c>
       <c r="Y166">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Z166">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="AA166">
         <v>-1</v>
       </c>
       <c r="AB166">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC166">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD166">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="167" spans="1:30">
@@ -16550,7 +16550,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>6832942</v>
+        <v>6832941</v>
       </c>
       <c r="C175" t="s">
         <v>29</v>
@@ -16559,79 +16559,79 @@
         <v>45382.22916666666</v>
       </c>
       <c r="E175" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F175" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G175">
+        <v>1</v>
+      </c>
+      <c r="H175">
         <v>3</v>
       </c>
-      <c r="H175">
-        <v>2</v>
-      </c>
       <c r="I175">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J175">
         <v>1</v>
       </c>
       <c r="K175" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L175">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="M175">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="N175">
-        <v>2.45</v>
+        <v>1.727</v>
       </c>
       <c r="O175">
-        <v>3.5</v>
+        <v>4.333</v>
       </c>
       <c r="P175">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="Q175">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="R175">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S175">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T175">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="U175">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="V175">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="W175">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="X175">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y175">
         <v>-1</v>
       </c>
       <c r="Z175">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA175">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB175">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC175">
-        <v>0.8999999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AD175">
         <v>-1</v>
@@ -16642,7 +16642,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>6832941</v>
+        <v>6832942</v>
       </c>
       <c r="C176" t="s">
         <v>29</v>
@@ -16651,79 +16651,79 @@
         <v>45382.22916666666</v>
       </c>
       <c r="E176" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F176" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G176">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H176">
+        <v>2</v>
+      </c>
+      <c r="I176">
         <v>3</v>
       </c>
-      <c r="I176">
-        <v>0</v>
-      </c>
       <c r="J176">
         <v>1</v>
       </c>
       <c r="K176" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L176">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="M176">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="N176">
-        <v>1.727</v>
+        <v>2.45</v>
       </c>
       <c r="O176">
-        <v>4.333</v>
+        <v>3.5</v>
       </c>
       <c r="P176">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="Q176">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="R176">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="S176">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T176">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="U176">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="V176">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="W176">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="X176">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y176">
         <v>-1</v>
       </c>
       <c r="Z176">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA176">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB176">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC176">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD176">
         <v>-1</v>
@@ -16826,7 +16826,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>6831810</v>
+        <v>6832950</v>
       </c>
       <c r="C178" t="s">
         <v>29</v>
@@ -16835,82 +16835,82 @@
         <v>45387.54861111111</v>
       </c>
       <c r="E178" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F178" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G178">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H178">
+        <v>1</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+      <c r="K178" t="s">
+        <v>50</v>
+      </c>
+      <c r="L178">
+        <v>2.05</v>
+      </c>
+      <c r="M178">
+        <v>3.6</v>
+      </c>
+      <c r="N178">
         <v>3</v>
       </c>
-      <c r="I178">
-        <v>1</v>
-      </c>
-      <c r="J178">
-        <v>2</v>
-      </c>
-      <c r="K178" t="s">
-        <v>52</v>
-      </c>
-      <c r="L178">
-        <v>5.25</v>
-      </c>
-      <c r="M178">
-        <v>3.75</v>
-      </c>
-      <c r="N178">
-        <v>1.6</v>
-      </c>
       <c r="O178">
-        <v>5.25</v>
+        <v>2.4</v>
       </c>
       <c r="P178">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="Q178">
-        <v>1.666</v>
+        <v>2.75</v>
       </c>
       <c r="R178">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S178">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="T178">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="U178">
         <v>2.75</v>
       </c>
       <c r="V178">
+        <v>1.75</v>
+      </c>
+      <c r="W178">
         <v>1.95</v>
       </c>
-      <c r="W178">
-        <v>1.85</v>
-      </c>
       <c r="X178">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y178">
         <v>-1</v>
       </c>
       <c r="Z178">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA178">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB178">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC178">
-        <v>0.95</v>
+        <v>0.375</v>
       </c>
       <c r="AD178">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="179" spans="1:30">
@@ -16918,7 +16918,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>6832947</v>
+        <v>6832949</v>
       </c>
       <c r="C179" t="s">
         <v>29</v>
@@ -16927,82 +16927,82 @@
         <v>45387.54861111111</v>
       </c>
       <c r="E179" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F179" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G179">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H179">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I179">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K179" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L179">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="M179">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="N179">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="O179">
-        <v>4</v>
+        <v>2.625</v>
       </c>
       <c r="P179">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="Q179">
+        <v>2.7</v>
+      </c>
+      <c r="R179">
+        <v>0</v>
+      </c>
+      <c r="S179">
+        <v>1.85</v>
+      </c>
+      <c r="T179">
+        <v>1.95</v>
+      </c>
+      <c r="U179">
+        <v>2.5</v>
+      </c>
+      <c r="V179">
         <v>1.8</v>
       </c>
-      <c r="R179">
-        <v>0.75</v>
-      </c>
-      <c r="S179">
-        <v>1.8</v>
-      </c>
-      <c r="T179">
-        <v>2</v>
-      </c>
-      <c r="U179">
-        <v>3</v>
-      </c>
-      <c r="V179">
-        <v>1.75</v>
-      </c>
       <c r="W179">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="X179">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="Y179">
         <v>-1</v>
       </c>
       <c r="Z179">
+        <v>-1</v>
+      </c>
+      <c r="AA179">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB179">
+        <v>-1</v>
+      </c>
+      <c r="AC179">
         <v>0.8</v>
       </c>
-      <c r="AA179">
-        <v>-0.5</v>
-      </c>
-      <c r="AB179">
-        <v>0.5</v>
-      </c>
-      <c r="AC179">
-        <v>0</v>
-      </c>
       <c r="AD179">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="180" spans="1:30">
@@ -17010,7 +17010,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>6832950</v>
+        <v>6831810</v>
       </c>
       <c r="C180" t="s">
         <v>29</v>
@@ -17019,82 +17019,82 @@
         <v>45387.54861111111</v>
       </c>
       <c r="E180" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F180" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G180">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H180">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J180">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K180" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L180">
-        <v>2.05</v>
+        <v>5.25</v>
       </c>
       <c r="M180">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="N180">
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="O180">
-        <v>2.4</v>
+        <v>5.25</v>
       </c>
       <c r="P180">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="Q180">
-        <v>2.75</v>
+        <v>1.666</v>
       </c>
       <c r="R180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S180">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="T180">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="U180">
         <v>2.75</v>
       </c>
       <c r="V180">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="W180">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="X180">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y180">
         <v>-1</v>
       </c>
       <c r="Z180">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="AA180">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB180">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AC180">
-        <v>0.375</v>
+        <v>0.95</v>
       </c>
       <c r="AD180">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="181" spans="1:30">
@@ -17102,7 +17102,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>6832949</v>
+        <v>6832947</v>
       </c>
       <c r="C181" t="s">
         <v>29</v>
@@ -17111,82 +17111,82 @@
         <v>45387.54861111111</v>
       </c>
       <c r="E181" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F181" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G181">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H181">
+        <v>2</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>1</v>
+      </c>
+      <c r="K181" t="s">
+        <v>52</v>
+      </c>
+      <c r="L181">
+        <v>4.2</v>
+      </c>
+      <c r="M181">
+        <v>4</v>
+      </c>
+      <c r="N181">
+        <v>1.7</v>
+      </c>
+      <c r="O181">
+        <v>4</v>
+      </c>
+      <c r="P181">
+        <v>4</v>
+      </c>
+      <c r="Q181">
+        <v>1.8</v>
+      </c>
+      <c r="R181">
+        <v>0.75</v>
+      </c>
+      <c r="S181">
+        <v>1.8</v>
+      </c>
+      <c r="T181">
+        <v>2</v>
+      </c>
+      <c r="U181">
         <v>3</v>
       </c>
-      <c r="I181">
-        <v>5</v>
-      </c>
-      <c r="J181">
-        <v>0</v>
-      </c>
-      <c r="K181" t="s">
-        <v>50</v>
-      </c>
-      <c r="L181">
-        <v>3.5</v>
-      </c>
-      <c r="M181">
-        <v>3.4</v>
-      </c>
-      <c r="N181">
+      <c r="V181">
+        <v>1.75</v>
+      </c>
+      <c r="W181">
         <v>1.95</v>
       </c>
-      <c r="O181">
-        <v>2.625</v>
-      </c>
-      <c r="P181">
-        <v>3.3</v>
-      </c>
-      <c r="Q181">
-        <v>2.7</v>
-      </c>
-      <c r="R181">
-        <v>0</v>
-      </c>
-      <c r="S181">
-        <v>1.85</v>
-      </c>
-      <c r="T181">
-        <v>1.95</v>
-      </c>
-      <c r="U181">
-        <v>2.5</v>
-      </c>
-      <c r="V181">
-        <v>1.8</v>
-      </c>
-      <c r="W181">
-        <v>2</v>
-      </c>
       <c r="X181">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="Y181">
         <v>-1</v>
       </c>
       <c r="Z181">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA181">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB181">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="AC181">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AD181">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:30">
@@ -19034,7 +19034,7 @@
         <v>200</v>
       </c>
       <c r="B202">
-        <v>6832964</v>
+        <v>6831812</v>
       </c>
       <c r="C202" t="s">
         <v>29</v>
@@ -19043,82 +19043,82 @@
         <v>45408.54861111111</v>
       </c>
       <c r="E202" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F202" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G202">
+        <v>1</v>
+      </c>
+      <c r="H202">
         <v>3</v>
       </c>
-      <c r="H202">
-        <v>0</v>
-      </c>
       <c r="I202">
+        <v>1</v>
+      </c>
+      <c r="J202">
+        <v>2</v>
+      </c>
+      <c r="K202" t="s">
+        <v>52</v>
+      </c>
+      <c r="L202">
+        <v>2.25</v>
+      </c>
+      <c r="M202">
+        <v>3.4</v>
+      </c>
+      <c r="N202">
+        <v>2.9</v>
+      </c>
+      <c r="O202">
+        <v>2.4</v>
+      </c>
+      <c r="P202">
+        <v>3.3</v>
+      </c>
+      <c r="Q202">
         <v>3</v>
       </c>
-      <c r="J202">
-        <v>0</v>
-      </c>
-      <c r="K202" t="s">
-        <v>50</v>
-      </c>
-      <c r="L202">
-        <v>1.4</v>
-      </c>
-      <c r="M202">
-        <v>5</v>
-      </c>
-      <c r="N202">
-        <v>6</v>
-      </c>
-      <c r="O202">
-        <v>1.3</v>
-      </c>
-      <c r="P202">
-        <v>5.5</v>
-      </c>
-      <c r="Q202">
-        <v>8.5</v>
-      </c>
       <c r="R202">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S202">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="T202">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="U202">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="V202">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W202">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X202">
-        <v>0.3</v>
+        <v>-1</v>
       </c>
       <c r="Y202">
         <v>-1</v>
       </c>
       <c r="Z202">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AA202">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB202">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AC202">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
       <c r="AD202">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="203" spans="1:30">
@@ -19126,7 +19126,7 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>6832109</v>
+        <v>6832964</v>
       </c>
       <c r="C203" t="s">
         <v>29</v>
@@ -19135,82 +19135,82 @@
         <v>45408.54861111111</v>
       </c>
       <c r="E203" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F203" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G203">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203">
         <v>3</v>
       </c>
-      <c r="I203">
-        <v>0</v>
-      </c>
       <c r="J203">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K203" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L203">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="M203">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="N203">
-        <v>1.8</v>
+        <v>6</v>
       </c>
       <c r="O203">
-        <v>4.333</v>
+        <v>1.3</v>
       </c>
       <c r="P203">
-        <v>3.4</v>
+        <v>5.5</v>
       </c>
       <c r="Q203">
-        <v>1.909</v>
+        <v>8.5</v>
       </c>
       <c r="R203">
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="S203">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="T203">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="U203">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="V203">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W203">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="X203">
-        <v>-1</v>
+        <v>0.3</v>
       </c>
       <c r="Y203">
         <v>-1</v>
       </c>
       <c r="Z203">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="AA203">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB203">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AC203">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AD203">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="204" spans="1:30">
@@ -19218,7 +19218,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>6831812</v>
+        <v>6832109</v>
       </c>
       <c r="C204" t="s">
         <v>29</v>
@@ -19227,61 +19227,61 @@
         <v>45408.54861111111</v>
       </c>
       <c r="E204" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F204" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G204">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H204">
         <v>3</v>
       </c>
       <c r="I204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J204">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K204" t="s">
         <v>52</v>
       </c>
       <c r="L204">
-        <v>2.25</v>
+        <v>4</v>
       </c>
       <c r="M204">
+        <v>3.6</v>
+      </c>
+      <c r="N204">
+        <v>1.8</v>
+      </c>
+      <c r="O204">
+        <v>4.333</v>
+      </c>
+      <c r="P204">
         <v>3.4</v>
       </c>
-      <c r="N204">
-        <v>2.9</v>
-      </c>
-      <c r="O204">
-        <v>2.4</v>
-      </c>
-      <c r="P204">
-        <v>3.3</v>
-      </c>
       <c r="Q204">
-        <v>3</v>
+        <v>1.909</v>
       </c>
       <c r="R204">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S204">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="T204">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="U204">
         <v>2.5</v>
       </c>
       <c r="V204">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W204">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="X204">
         <v>-1</v>
@@ -19290,16 +19290,16 @@
         <v>-1</v>
       </c>
       <c r="Z204">
-        <v>2</v>
+        <v>0.909</v>
       </c>
       <c r="AA204">
         <v>-1</v>
       </c>
       <c r="AB204">
-        <v>0.7749999999999999</v>
+        <v>0.875</v>
       </c>
       <c r="AC204">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="AD204">
         <v>-1</v>
@@ -22438,7 +22438,7 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>6832982</v>
+        <v>6832981</v>
       </c>
       <c r="C239" t="s">
         <v>29</v>
@@ -22447,82 +22447,82 @@
         <v>45432.45833333334</v>
       </c>
       <c r="E239" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F239" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H239">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J239">
         <v>0</v>
       </c>
       <c r="K239" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L239">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="M239">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="N239">
-        <v>1.909</v>
+        <v>2</v>
       </c>
       <c r="O239">
-        <v>2.75</v>
+        <v>2.9</v>
       </c>
       <c r="P239">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="Q239">
-        <v>2.4</v>
+        <v>2.15</v>
       </c>
       <c r="R239">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S239">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T239">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="U239">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="V239">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W239">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="X239">
         <v>-1</v>
       </c>
       <c r="Y239">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z239">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="AA239">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB239">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC239">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AD239">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="240" spans="1:30">
@@ -22530,7 +22530,7 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>6832981</v>
+        <v>6832982</v>
       </c>
       <c r="C240" t="s">
         <v>29</v>
@@ -22539,82 +22539,82 @@
         <v>45432.45833333334</v>
       </c>
       <c r="E240" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F240" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H240">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J240">
         <v>0</v>
       </c>
       <c r="K240" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L240">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="M240">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="N240">
-        <v>2</v>
+        <v>1.909</v>
       </c>
       <c r="O240">
-        <v>2.9</v>
+        <v>2.75</v>
       </c>
       <c r="P240">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="Q240">
-        <v>2.15</v>
+        <v>2.4</v>
       </c>
       <c r="R240">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S240">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="T240">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="U240">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="V240">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W240">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="X240">
         <v>-1</v>
       </c>
       <c r="Y240">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z240">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="AA240">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB240">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AC240">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD240">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="241" spans="1:30">

</xml_diff>